<commit_message>
Reporte de plenarias completado
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-reportes-plenarias.xlsx
+++ b/assets/info/plantilla-reportes-plenarias.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t xml:space="preserve">REPORTE AGENDA LEGISLATIVA</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONITOR</t>
   </si>
   <si>
     <t xml:space="preserve">REPORTES NOTICIAS</t>
@@ -363,9 +366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>986400</xdr:colOff>
+      <xdr:colOff>986040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -379,7 +382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="314640"/>
-          <a:ext cx="3589920" cy="1122840"/>
+          <a:ext cx="3589560" cy="1122480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -405,9 +408,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>919800</xdr:colOff>
+      <xdr:colOff>919440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,7 +424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3523320" cy="1256400"/>
+          <a:ext cx="3522960" cy="1256040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -447,9 +450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>729000</xdr:colOff>
+      <xdr:colOff>728640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>227520</xdr:rowOff>
+      <xdr:rowOff>227160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -463,7 +466,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3332520" cy="1303920"/>
+          <a:ext cx="3332160" cy="1303560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -485,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,7 +581,9 @@
       <c r="M5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="10"/>
+      <c r="N5" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="O5" s="10"/>
     </row>
   </sheetData>
@@ -649,7 +654,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -684,22 +689,22 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -777,7 +782,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -812,25 +817,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>

</xml_diff>